<commit_message>
Update USB connector: Create component and update schematics as well
</commit_message>
<xml_diff>
--- a/Connect Medical Boards/EFM1/Project Outputs for 105358-3BA001-01_EFM1/105358-3BA001-01_EFM1_BOM.xlsx
+++ b/Connect Medical Boards/EFM1/Project Outputs for 105358-3BA001-01_EFM1/105358-3BA001-01_EFM1_BOM.xlsx
@@ -147,13 +147,13 @@
     <t>USB Micro B</t>
   </si>
   <si>
-    <t>DX4R005JJ7R1500</t>
-  </si>
-  <si>
-    <t>JAE Electronics</t>
-  </si>
-  <si>
-    <t>670-2678-1-ND</t>
+    <t>UJ2-MIBH-4-MSMT-TR</t>
+  </si>
+  <si>
+    <t>CUI Inc.</t>
+  </si>
+  <si>
+    <t>102-4008-1-ND</t>
   </si>
   <si>
     <t>CON2</t>

</xml_diff>

<commit_message>
- Update component so Digi-Key Part Number use multiples of 1K to buy - Separate component 0603 10uF into 10uF-4V and 10uF-10V - Update Schematics - Update BOM and BOM cost
</commit_message>
<xml_diff>
--- a/Connect Medical Boards/EFM1/Project Outputs for 105358-3BA001-01_EFM1/105358-3BA001-01_EFM1_BOM.xlsx
+++ b/Connect Medical Boards/EFM1/Project Outputs for 105358-3BA001-01_EFM1/105358-3BA001-01_EFM1_BOM.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Connect Medical Boards\EFM1\Project Outputs for 105358-3BA001-01_EFM1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11595"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="150">
   <si>
     <t>Designator</t>
   </si>
@@ -108,22 +113,37 @@
     <t>445-5947-1-ND</t>
   </si>
   <si>
-    <t>C4, C5, C6</t>
-  </si>
-  <si>
-    <t>10µF ±10% 4V X6S Ceramic Capacitor 0603, 10µF ±10% 10V X5R Ceramic Capacitor 0603, 10µF ±10% 10V X5R Ceramic Capacitor 0603</t>
-  </si>
-  <si>
-    <t>10µF</t>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>10µF ±10% 4V X6S Ceramic Capacitor 0603</t>
+  </si>
+  <si>
+    <t>10µF-4V</t>
   </si>
   <si>
     <t>Murata Electronics North America</t>
   </si>
   <si>
-    <t>GRM188C80G106KE47D, GRM188R61A106KE69D, GRM188R61A106KE69D</t>
-  </si>
-  <si>
-    <t>490-10469-1-ND, 490-10474-1-ND, 490-10474-1-ND</t>
+    <t>GRM188C80G106KE47D</t>
+  </si>
+  <si>
+    <t>490-10469-1-ND</t>
+  </si>
+  <si>
+    <t>C5, C6</t>
+  </si>
+  <si>
+    <t>10µF ±10% 10V X5R Ceramic Capacitor 0603</t>
+  </si>
+  <si>
+    <t>10µF-10V</t>
+  </si>
+  <si>
+    <t>GRM188R61A106KE69D</t>
+  </si>
+  <si>
+    <t>490-10474-1-ND</t>
   </si>
   <si>
     <t>C13</t>
@@ -168,7 +188,7 @@
     <t>Molex, LLC</t>
   </si>
   <si>
-    <t>WM4459TR-ND</t>
+    <t>WM4459CT-ND</t>
   </si>
   <si>
     <t>D1</t>
@@ -213,7 +233,7 @@
     <t>MLZ2012N150LT000</t>
   </si>
   <si>
-    <t>445-6763-2-ND</t>
+    <t>445-6763-1-ND</t>
   </si>
   <si>
     <t>0805</t>
@@ -231,7 +251,7 @@
     <t>MLZ2012M2R2HTD25</t>
   </si>
   <si>
-    <t>445-17077-2-ND</t>
+    <t>445-17077-1-ND</t>
   </si>
   <si>
     <t>L3</t>
@@ -399,7 +419,7 @@
     <t>TPS627431YFPR</t>
   </si>
   <si>
-    <t>296-44499-1-ND</t>
+    <t>296-44499-2-ND</t>
   </si>
   <si>
     <t>8-XFBGA, DSBGA</t>
@@ -803,9 +823,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -958,7 +980,7 @@
         <v>22</v>
       </c>
       <c r="H5" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>16</v>
@@ -984,10 +1006,10 @@
         <v>39</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>16</v>
@@ -1004,16 +1026,16 @@
         <v>42</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7" s="3">
         <v>1</v>
@@ -1071,7 +1093,7 @@
         <v>54</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H9" s="3">
         <v>1</v>
@@ -1100,7 +1122,7 @@
         <v>59</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H10" s="3">
         <v>1</v>
@@ -1120,16 +1142,16 @@
         <v>62</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>64</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="H11" s="3">
         <v>1</v>
@@ -1140,25 +1162,25 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="H12" s="3">
         <v>1</v>
@@ -1178,16 +1200,16 @@
         <v>73</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H13" s="3">
         <v>1</v>
@@ -1207,16 +1229,16 @@
         <v>78</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
@@ -1236,16 +1258,16 @@
         <v>83</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="H15" s="3">
         <v>1</v>
@@ -1256,60 +1278,60 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="G16" s="2" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="H16" s="3">
         <v>1</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H17" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1323,7 +1345,7 @@
         <v>99</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>100</v>
@@ -1335,10 +1357,10 @@
         <v>15</v>
       </c>
       <c r="H18" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1352,7 +1374,7 @@
         <v>104</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>105</v>
@@ -1367,7 +1389,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1381,7 +1403,7 @@
         <v>109</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>110</v>
@@ -1396,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1410,7 +1432,7 @@
         <v>114</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>115</v>
@@ -1425,7 +1447,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1439,39 +1461,39 @@
         <v>119</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>121</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>122</v>
+        <v>15</v>
       </c>
       <c r="H22" s="3">
         <v>1</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>126</v>
@@ -1497,7 +1519,7 @@
         <v>130</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>130</v>
@@ -1526,16 +1548,16 @@
         <v>135</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F25" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="H25" s="3">
         <v>1</v>
@@ -1546,30 +1568,59 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="3">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H26" s="3">
-        <v>1</v>
-      </c>
-      <c r="I26" s="2" t="s">
+      <c r="B27" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>